<commit_message>
tried a different way
</commit_message>
<xml_diff>
--- a/part-1.xlsx
+++ b/part-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sabrina/Downloads/ps1-vector-space-model-swong040/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A445C9D-A38C-6643-B301-E17756D9BE45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2858370-F340-044A-83EF-CB6CBC152E8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{384D9387-6084-1042-AEE6-6BE5728690FD}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{384D9387-6084-1042-AEE6-6BE5728690FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="d6_tot">Sheet1!$Q$16</definedName>
     <definedName name="d7_tot">Sheet1!$Q$17</definedName>
     <definedName name="d8_tot">Sheet1!$Q$18</definedName>
-    <definedName name="totTerms">Sheet1!$B$81</definedName>
+    <definedName name="totTerms">Sheet1!$B$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -588,7 +588,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -628,6 +628,12 @@
       <color theme="1"/>
       <name val="CMEX10"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -649,13 +655,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C187F34D-70DE-3A4B-8197-7EC6DB94C321}">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -988,9 +995,6 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="2" spans="1:17">
       <c r="C2" t="s">
@@ -1021,7 +1025,7 @@
         <v>75</v>
       </c>
       <c r="N2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1036,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1051,7 +1055,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1066,7 +1070,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1081,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1095,6 +1099,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:17">
       <c r="B8" t="s">
@@ -1153,8 +1160,8 @@
         <v>67</v>
       </c>
       <c r="Q11">
-        <f>IF(LEN(TRIM(N11))=0,0,LEN(TRIM(N11))-LEN(SUBSTITUTE(N11," ",""))+1)</f>
-        <v>7</v>
+        <f>IF(LEN(TRIM(N11))=0,0,LEN(TRIM(N11))-LEN(SUBSTITUTE(N11," ",""))+1)-2</f>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1175,8 +1182,8 @@
         <v>68</v>
       </c>
       <c r="Q12">
-        <f t="shared" ref="Q12:Q18" si="1">IF(LEN(TRIM(N12))=0,0,LEN(TRIM(N12))-LEN(SUBSTITUTE(N12," ",""))+1)</f>
-        <v>6</v>
+        <f>IF(LEN(TRIM(N12))=0,0,LEN(TRIM(N12))-LEN(SUBSTITUTE(N12," ",""))+1)-3</f>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1197,8 +1204,8 @@
         <v>69</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>IF(LEN(TRIM(N13))=0,0,LEN(TRIM(N13))-LEN(SUBSTITUTE(N13," ",""))+1)-1</f>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1219,8 +1226,8 @@
         <v>70</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f>IF(LEN(TRIM(N14))=0,0,LEN(TRIM(N14))-LEN(SUBSTITUTE(N14," ",""))+1)-1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1241,8 +1248,8 @@
         <v>71</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>IF(LEN(TRIM(N15))=0,0,LEN(TRIM(N15))-LEN(SUBSTITUTE(N15," ",""))+1)-1</f>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1263,7 +1270,7 @@
         <v>72</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="1"/>
+        <f>IF(LEN(TRIM(N16))=0,0,LEN(TRIM(N16))-LEN(SUBSTITUTE(N16," ",""))+1)</f>
         <v>6</v>
       </c>
     </row>
@@ -1285,8 +1292,8 @@
         <v>73</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f>IF(LEN(TRIM(N17))=0,0,LEN(TRIM(N17))-LEN(SUBSTITUTE(N17," ",""))+1)-1</f>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:17">
@@ -1307,8 +1314,8 @@
         <v>74</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f>IF(LEN(TRIM(N18))=0,0,LEN(TRIM(N18))-LEN(SUBSTITUTE(N18," ",""))+1)-1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:17">
@@ -1643,1606 +1650,1600 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="5">
+    <row r="45" spans="1:13">
+      <c r="A45" s="5">
         <v>5</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="5"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K45" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M45" t="s">
-        <v>57</v>
-      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="5"/>
-      <c r="B46" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="5">
-        <f>C3/d1_tot</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="5">
-        <f>D3/d2_tot</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="5">
-        <f t="shared" ref="E46:E80" si="2">E3/d3_tot</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="5">
-        <f t="shared" ref="F46:F80" si="3">F3/d4_tot</f>
-        <v>0.2</v>
-      </c>
-      <c r="G46" s="5">
-        <f t="shared" ref="G46:G80" si="4">G3/d5_tot</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="5">
-        <f t="shared" ref="H46:H80" si="5">H3/d6_tot</f>
-        <v>0</v>
-      </c>
-      <c r="I46" s="5">
-        <f t="shared" ref="I46:I80" si="6">I3/d7_tot</f>
-        <v>0</v>
-      </c>
-      <c r="J46" s="5">
-        <f t="shared" ref="J46:J80" si="7">J3/d8_tot</f>
-        <v>0</v>
-      </c>
-      <c r="K46" s="5">
-        <f>LOG(8/K3,2)</f>
-        <v>3</v>
-      </c>
-      <c r="L46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="M46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" ref="C47:C80" si="8">C4/d1_tot</f>
+        <f>C3/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D47" s="5">
-        <f t="shared" ref="D47:D80" si="9">D4/d2_tot</f>
+        <f>D3/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" si="2"/>
+        <f>E3/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F47" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>F3/d4_tot</f>
+        <v>0.25</v>
       </c>
       <c r="G47" s="5">
-        <f t="shared" si="4"/>
+        <f>G3/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H47" s="5">
-        <f t="shared" si="5"/>
-        <v>0.16666666666666666</v>
+        <f>H3/d6_tot</f>
+        <v>0</v>
       </c>
       <c r="I47" s="5">
-        <f t="shared" si="6"/>
+        <f>I3/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J47" s="5">
-        <f t="shared" si="7"/>
+        <f>J3/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K47" s="5">
-        <f t="shared" ref="K47:K80" si="10">LOG(8/K4,2)</f>
-        <v>3</v>
+        <f>LN(8/K3)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L47" s="5"/>
+      <c r="M47" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="8"/>
+        <f>C4/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D48" s="5">
-        <f t="shared" si="9"/>
+        <f>D4/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E48" s="5">
-        <f t="shared" si="2"/>
-        <v>0.14285714285714285</v>
+        <f>E4/d3_tot</f>
+        <v>0</v>
       </c>
       <c r="F48" s="5">
-        <f t="shared" si="3"/>
+        <f>F4/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G48" s="5">
-        <f t="shared" si="4"/>
+        <f>G4/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H48" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>H4/d6_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I48" s="5">
-        <f t="shared" si="6"/>
+        <f>I4/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J48" s="5">
-        <f t="shared" si="7"/>
+        <f>J4/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K48" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K4)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:12">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="8"/>
+        <f>C5/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D49" s="5">
-        <f t="shared" si="9"/>
+        <f>D5/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E49" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>E5/d3_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F49" s="5">
-        <f t="shared" si="3"/>
+        <f>F5/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G49" s="5">
-        <f t="shared" si="4"/>
+        <f>G5/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H49" s="5">
-        <f t="shared" si="5"/>
+        <f>H5/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I49" s="5">
-        <f t="shared" si="6"/>
+        <f>I5/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J49" s="5">
-        <f t="shared" si="7"/>
-        <v>0.2</v>
+        <f>J5/d8_tot</f>
+        <v>0</v>
       </c>
       <c r="K49" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K5)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L49" s="5"/>
-      <c r="O49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15">
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="5"/>
       <c r="B50" s="5" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="8"/>
+        <f>C6/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D50" s="5">
-        <f t="shared" si="9"/>
+        <f>D6/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E50" s="5">
-        <f t="shared" si="2"/>
+        <f>E6/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F50" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
+        <f>F6/d4_tot</f>
+        <v>0</v>
       </c>
       <c r="G50" s="5">
-        <f t="shared" si="4"/>
+        <f>G6/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H50" s="5">
-        <f t="shared" si="5"/>
+        <f>H6/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I50" s="5">
-        <f t="shared" si="6"/>
+        <f>I6/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J50" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>J6/d8_tot</f>
+        <v>0.25</v>
       </c>
       <c r="K50" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K6)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L50" s="5"/>
-      <c r="O50" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15">
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="8"/>
+        <f>C7/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D51" s="5">
-        <f t="shared" si="9"/>
+        <f>D7/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E51" s="5">
-        <f t="shared" si="2"/>
+        <f>E7/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F51" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>F7/d4_tot</f>
+        <v>0.25</v>
       </c>
       <c r="G51" s="5">
-        <f t="shared" si="4"/>
+        <f>G7/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H51" s="5">
-        <f t="shared" si="5"/>
-        <v>0.16666666666666666</v>
+        <f>H7/d6_tot</f>
+        <v>0</v>
       </c>
       <c r="I51" s="5">
-        <f t="shared" si="6"/>
+        <f>I7/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="7"/>
+        <f>J7/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K51" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K7)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:12">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="8"/>
+        <f>C8/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D52" s="5">
-        <f t="shared" si="9"/>
+        <f>D8/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E52" s="5">
-        <f t="shared" si="2"/>
+        <f>E8/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F52" s="5">
-        <f t="shared" si="3"/>
+        <f>F8/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G52" s="5">
-        <f t="shared" si="4"/>
+        <f>G8/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H52" s="5">
-        <f t="shared" si="5"/>
+        <f>H8/d6_tot</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="I52" s="5">
-        <f t="shared" si="6"/>
+        <f>I8/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J52" s="5">
-        <f t="shared" si="7"/>
+        <f>J8/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K52" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K8)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:12">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="8"/>
+        <f>C9/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D53" s="5">
-        <f t="shared" si="9"/>
+        <f>D9/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E53" s="5">
-        <f t="shared" si="2"/>
-        <v>0.14285714285714285</v>
+        <f>E9/d3_tot</f>
+        <v>0</v>
       </c>
       <c r="F53" s="5">
-        <f t="shared" si="3"/>
+        <f>F9/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G53" s="5">
-        <f t="shared" si="4"/>
+        <f>G9/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H53" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>H9/d6_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I53" s="5">
-        <f t="shared" si="6"/>
+        <f>I9/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J53" s="5">
-        <f t="shared" si="7"/>
+        <f>J9/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K53" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K9)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:12">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="8"/>
+        <f>C10/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D54" s="5">
-        <f t="shared" si="9"/>
+        <f>D10/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E54" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>E10/d3_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F54" s="5">
-        <f t="shared" si="3"/>
+        <f>F10/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G54" s="5">
-        <f t="shared" si="4"/>
+        <f>G10/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H54" s="5">
-        <f t="shared" si="5"/>
+        <f>H10/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I54" s="5">
-        <f t="shared" si="6"/>
-        <v>0.125</v>
+        <f>I10/d7_tot</f>
+        <v>0</v>
       </c>
       <c r="J54" s="5">
-        <f t="shared" si="7"/>
+        <f>J10/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K54" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K10)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:12">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="8"/>
+        <f>C11/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D55" s="5">
-        <f t="shared" si="9"/>
+        <f>D11/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E55" s="5">
-        <f t="shared" si="2"/>
+        <f>E11/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F55" s="5">
-        <f t="shared" si="3"/>
+        <f>F11/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G55" s="5">
-        <f t="shared" si="4"/>
+        <f>G11/d5_tot</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="5">
+        <f>H11/d6_tot</f>
+        <v>0</v>
+      </c>
+      <c r="I55" s="5">
+        <f>I11/d7_tot</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="H55" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I55" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="J55" s="5">
-        <f t="shared" si="7"/>
+        <f>J11/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K55" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K11)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:12">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="8"/>
+        <f>C12/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D56" s="5">
-        <f t="shared" si="9"/>
+        <f>D12/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E56" s="5">
-        <f t="shared" si="2"/>
+        <f>E12/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F56" s="5">
-        <f t="shared" si="3"/>
+        <f>F12/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G56" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>G12/d5_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H56" s="5">
-        <f t="shared" si="5"/>
+        <f>H12/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I56" s="5">
-        <f t="shared" si="6"/>
-        <v>0.125</v>
+        <f>I12/d7_tot</f>
+        <v>0</v>
       </c>
       <c r="J56" s="5">
-        <f t="shared" si="7"/>
+        <f>J12/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K56" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K12)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:12">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="8"/>
+        <f>C13/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D57" s="5">
-        <f t="shared" si="9"/>
+        <f>D13/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E57" s="5">
-        <f t="shared" si="2"/>
+        <f>E13/d3_tot</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="5">
+        <f>F13/d4_tot</f>
+        <v>0</v>
+      </c>
+      <c r="G57" s="5">
+        <f>G13/d5_tot</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="5">
+        <f>H13/d6_tot</f>
+        <v>0</v>
+      </c>
+      <c r="I57" s="5">
+        <f>I13/d7_tot</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="F57" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G57" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H57" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I57" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="J57" s="5">
-        <f t="shared" si="7"/>
+        <f>J13/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K57" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K13)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:12">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="8"/>
+        <f>C14/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D58" s="5">
-        <f t="shared" si="9"/>
+        <f>D14/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E58" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>E14/d3_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F58" s="5">
-        <f t="shared" si="3"/>
+        <f>F14/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G58" s="5">
-        <f t="shared" si="4"/>
+        <f>G14/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H58" s="5">
-        <f t="shared" si="5"/>
-        <v>0.16666666666666666</v>
+        <f>H14/d6_tot</f>
+        <v>0</v>
       </c>
       <c r="I58" s="5">
-        <f t="shared" si="6"/>
+        <f>I14/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J58" s="5">
-        <f t="shared" si="7"/>
+        <f>J14/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K58" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K14)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:12">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="8"/>
+        <f>C15/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D59" s="5">
-        <f t="shared" si="9"/>
+        <f>D15/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E59" s="5">
-        <f t="shared" si="2"/>
-        <v>0.14285714285714285</v>
+        <f>E15/d3_tot</f>
+        <v>0</v>
       </c>
       <c r="F59" s="5">
-        <f t="shared" si="3"/>
+        <f>F15/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G59" s="5">
-        <f t="shared" si="4"/>
+        <f>G15/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H59" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>H15/d6_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I59" s="5">
-        <f t="shared" si="6"/>
+        <f>I15/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J59" s="5">
-        <f t="shared" si="7"/>
+        <f>J15/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K59" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K15)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:12">
       <c r="A60" s="5"/>
       <c r="B60" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="8"/>
+        <f>C16/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D60" s="5">
-        <f t="shared" si="9"/>
+        <f>D16/d2_tot</f>
+        <v>0</v>
+      </c>
+      <c r="E60" s="5">
+        <f>E16/d3_tot</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E60" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="F60" s="5">
-        <f t="shared" si="3"/>
+        <f>F16/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G60" s="5">
-        <f t="shared" si="4"/>
+        <f>G16/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H60" s="5">
-        <f t="shared" si="5"/>
+        <f>H16/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I60" s="5">
-        <f t="shared" si="6"/>
+        <f>I16/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J60" s="5">
-        <f t="shared" si="7"/>
+        <f>J16/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K60" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K16)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:12">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="8"/>
+        <f>C17/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D61" s="5">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>D17/d2_tot</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E61" s="5">
-        <f t="shared" si="2"/>
+        <f>E17/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F61" s="5">
-        <f t="shared" si="3"/>
+        <f>F17/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G61" s="5">
-        <f t="shared" si="4"/>
-        <v>0.14285714285714285</v>
+        <f>G17/d5_tot</f>
+        <v>0</v>
       </c>
       <c r="H61" s="5">
-        <f t="shared" si="5"/>
+        <f>H17/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I61" s="5">
-        <f t="shared" si="6"/>
+        <f>I17/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J61" s="5">
-        <f t="shared" si="7"/>
+        <f>J17/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K61" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K17)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:12">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="8"/>
+        <f>C18/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D62" s="5">
-        <f t="shared" si="9"/>
+        <f>D18/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E62" s="5">
-        <f t="shared" si="2"/>
+        <f>E18/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F62" s="5">
-        <f t="shared" si="3"/>
+        <f>F18/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G62" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>G18/d5_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H62" s="5">
-        <f t="shared" si="5"/>
-        <v>0.16666666666666666</v>
+        <f>H18/d6_tot</f>
+        <v>0</v>
       </c>
       <c r="I62" s="5">
-        <f t="shared" si="6"/>
+        <f>I18/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J62" s="5">
-        <f t="shared" si="7"/>
+        <f>J18/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K62" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K18)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:12">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
+        <f>C19/d1_tot</f>
+        <v>0</v>
       </c>
       <c r="D63" s="5">
-        <f t="shared" si="9"/>
+        <f>D19/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E63" s="5">
-        <f t="shared" si="2"/>
+        <f>E19/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F63" s="5">
-        <f t="shared" si="3"/>
+        <f>F19/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G63" s="5">
-        <f t="shared" si="4"/>
+        <f>G19/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H63" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>H19/d6_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I63" s="5">
-        <f t="shared" si="6"/>
+        <f>I19/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J63" s="5">
-        <f t="shared" si="7"/>
+        <f>J19/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K63" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="L63" s="5">
-        <f>C63*K63</f>
-        <v>0.42857142857142855</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15">
+        <f>LN(8/K19)</f>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L63" s="5"/>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>C20/d1_tot</f>
+        <v>0.2</v>
       </c>
       <c r="D64" s="5">
-        <f t="shared" si="9"/>
+        <f>D20/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E64" s="5">
-        <f t="shared" si="2"/>
-        <v>0.14285714285714285</v>
+        <f>E20/d3_tot</f>
+        <v>0</v>
       </c>
       <c r="F64" s="5">
-        <f t="shared" si="3"/>
+        <f>F20/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G64" s="5">
-        <f t="shared" si="4"/>
+        <f>G20/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H64" s="5">
-        <f t="shared" si="5"/>
+        <f>H20/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I64" s="5">
-        <f t="shared" si="6"/>
-        <v>0.125</v>
+        <f>I20/d7_tot</f>
+        <v>0</v>
       </c>
       <c r="J64" s="5">
-        <f t="shared" si="7"/>
+        <f>J20/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K64" s="5">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="L64" s="5"/>
+        <f>LN(8/K20)</f>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L64" s="5">
+        <f>C64*K64</f>
+        <v>0.41588830833596718</v>
+      </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="8"/>
+        <f>C21/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D65" s="5">
-        <f t="shared" si="9"/>
+        <f>D21/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E65" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>E21/d3_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F65" s="5">
-        <f t="shared" si="3"/>
+        <f>F21/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G65" s="5">
-        <f t="shared" si="4"/>
+        <f>G21/d5_tot</f>
+        <v>0</v>
+      </c>
+      <c r="H65" s="5">
+        <f>H21/d6_tot</f>
+        <v>0</v>
+      </c>
+      <c r="I65" s="5">
+        <f>I21/d7_tot</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="H65" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I65" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="J65" s="5">
-        <f t="shared" si="7"/>
+        <f>J21/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K65" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K21)</f>
+        <v>1.3862943611198906</v>
       </c>
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
+        <f>C22/d1_tot</f>
+        <v>0</v>
       </c>
       <c r="D66" s="5">
-        <f t="shared" si="9"/>
+        <f>D22/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E66" s="5">
-        <f t="shared" si="2"/>
-        <v>0.14285714285714285</v>
+        <f>E22/d3_tot</f>
+        <v>0</v>
       </c>
       <c r="F66" s="5">
-        <f t="shared" si="3"/>
+        <f>F22/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G66" s="5">
-        <f t="shared" si="4"/>
-        <v>0.14285714285714285</v>
+        <f>G22/d5_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H66" s="5">
-        <f t="shared" si="5"/>
+        <f>H22/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I66" s="5">
-        <f t="shared" si="6"/>
+        <f>I22/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J66" s="5">
-        <f t="shared" si="7"/>
+        <f>J22/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K66" s="5">
-        <f t="shared" si="10"/>
-        <v>1.4150374992788437</v>
-      </c>
-      <c r="L66" s="5">
-        <f>C66*K66</f>
-        <v>0.20214821418269194</v>
-      </c>
+        <f>LN(8/K22)</f>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L66" s="5"/>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
+        <f>C23/d1_tot</f>
+        <v>0.2</v>
       </c>
       <c r="D67" s="5">
-        <f t="shared" si="9"/>
+        <f>D23/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E67" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>E23/d3_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F67" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
+        <f>F23/d4_tot</f>
+        <v>0</v>
       </c>
       <c r="G67" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>G23/d5_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H67" s="5">
-        <f t="shared" si="5"/>
+        <f>H23/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I67" s="5">
-        <f t="shared" si="6"/>
+        <f>I23/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J67" s="5">
-        <f t="shared" si="7"/>
+        <f>J23/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K67" s="5">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>LN(8/K23)</f>
+        <v>0.98082925301172619</v>
       </c>
       <c r="L67" s="5">
         <f>C67*K67</f>
-        <v>0.2857142857142857</v>
+        <v>0.19616585060234526</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="5"/>
       <c r="B68" s="5" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>C24/d1_tot</f>
+        <v>0.2</v>
       </c>
       <c r="D68" s="5">
-        <f t="shared" si="9"/>
+        <f>D24/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E68" s="5">
-        <f t="shared" si="2"/>
+        <f>E24/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F68" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>F24/d4_tot</f>
+        <v>0.25</v>
       </c>
       <c r="G68" s="5">
-        <f t="shared" si="4"/>
+        <f>G24/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H68" s="5">
-        <f t="shared" si="5"/>
+        <f>H24/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I68" s="5">
-        <f t="shared" si="6"/>
-        <v>0.125</v>
+        <f>I24/d7_tot</f>
+        <v>0</v>
       </c>
       <c r="J68" s="5">
-        <f t="shared" si="7"/>
+        <f>J24/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K68" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="L68" s="5"/>
+        <f>LN(8/K24)</f>
+        <v>1.3862943611198906</v>
+      </c>
+      <c r="L68" s="5">
+        <f>C68*K68</f>
+        <v>0.2772588722239781</v>
+      </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="5"/>
       <c r="B69" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C69" s="5">
-        <f t="shared" si="8"/>
+        <f>C25/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D69" s="5">
-        <f t="shared" si="9"/>
+        <f>D25/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E69" s="5">
-        <f t="shared" si="2"/>
+        <f>E25/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F69" s="5">
-        <f t="shared" si="3"/>
+        <f>F25/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G69" s="5">
-        <f t="shared" si="4"/>
+        <f>G25/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H69" s="5">
-        <f t="shared" si="5"/>
+        <f>H25/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I69" s="5">
-        <f t="shared" si="6"/>
-        <v>0.125</v>
+        <f>I25/d7_tot</f>
+        <v>0.14285714285714285</v>
       </c>
       <c r="J69" s="5">
-        <f t="shared" si="7"/>
+        <f>J25/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K69" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K25)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L69" s="5"/>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="5"/>
       <c r="B70" s="5" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" si="8"/>
+        <f>C26/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D70" s="5">
-        <f t="shared" si="9"/>
-        <v>0.16666666666666666</v>
+        <f>D26/d2_tot</f>
+        <v>0</v>
       </c>
       <c r="E70" s="5">
-        <f t="shared" si="2"/>
+        <f>E26/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F70" s="5">
-        <f t="shared" si="3"/>
+        <f>F26/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G70" s="5">
-        <f t="shared" si="4"/>
+        <f>G26/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H70" s="5">
-        <f t="shared" si="5"/>
+        <f>H26/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I70" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>I26/d7_tot</f>
+        <v>0.14285714285714285</v>
       </c>
       <c r="J70" s="5">
-        <f t="shared" si="7"/>
+        <f>J26/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K70" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K26)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L70" s="5"/>
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="5"/>
       <c r="B71" s="5" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C71" s="5">
-        <f t="shared" si="8"/>
+        <f>C27/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D71" s="5">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>D27/d2_tot</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E71" s="5">
-        <f t="shared" si="2"/>
+        <f>E27/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F71" s="5">
-        <f t="shared" si="3"/>
+        <f>F27/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G71" s="5">
-        <f t="shared" si="4"/>
+        <f>G27/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H71" s="5">
-        <f t="shared" si="5"/>
+        <f>H27/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I71" s="5">
-        <f t="shared" si="6"/>
+        <f>I27/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J71" s="5">
-        <f t="shared" si="7"/>
-        <v>0.2</v>
+        <f>J27/d8_tot</f>
+        <v>0</v>
       </c>
       <c r="K71" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K27)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L71" s="5"/>
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C72" s="5">
-        <f t="shared" si="8"/>
+        <f>C28/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D72" s="5">
-        <f t="shared" si="9"/>
+        <f>D28/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E72" s="5">
-        <f t="shared" si="2"/>
+        <f>E28/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F72" s="5">
-        <f t="shared" si="3"/>
+        <f>F28/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G72" s="5">
-        <f t="shared" si="4"/>
+        <f>G28/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H72" s="5">
-        <f t="shared" si="5"/>
+        <f>H28/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I72" s="5">
-        <f t="shared" si="6"/>
-        <v>0.125</v>
+        <f>I28/d7_tot</f>
+        <v>0</v>
       </c>
       <c r="J72" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>J28/d8_tot</f>
+        <v>0.25</v>
       </c>
       <c r="K72" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K28)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L72" s="5"/>
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C73" s="5">
-        <f t="shared" si="8"/>
+        <f>C29/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D73" s="5">
-        <f t="shared" si="9"/>
+        <f>D29/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E73" s="5">
-        <f t="shared" si="2"/>
+        <f>E29/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F73" s="5">
-        <f t="shared" si="3"/>
+        <f>F29/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G73" s="5">
-        <f t="shared" si="4"/>
+        <f>G29/d5_tot</f>
+        <v>0</v>
+      </c>
+      <c r="H73" s="5">
+        <f>H29/d6_tot</f>
+        <v>0</v>
+      </c>
+      <c r="I73" s="5">
+        <f>I29/d7_tot</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="H73" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I73" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="J73" s="5">
-        <f t="shared" si="7"/>
+        <f>J29/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K73" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K29)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L73" s="5"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C74" s="5">
-        <f t="shared" si="8"/>
+        <f>C30/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D74" s="5">
-        <f t="shared" si="9"/>
+        <f>D30/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E74" s="5">
-        <f t="shared" si="2"/>
+        <f>E30/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F74" s="5">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
+        <f>F30/d4_tot</f>
+        <v>0</v>
       </c>
       <c r="G74" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>G30/d5_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H74" s="5">
-        <f t="shared" si="5"/>
+        <f>H30/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I74" s="5">
-        <f t="shared" si="6"/>
+        <f>I30/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J74" s="5">
-        <f t="shared" si="7"/>
+        <f>J30/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K74" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K30)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L74" s="5"/>
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C75" s="5">
-        <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
+        <f>C31/d1_tot</f>
+        <v>0</v>
       </c>
       <c r="D75" s="5">
-        <f t="shared" si="9"/>
+        <f>D31/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E75" s="5">
-        <f t="shared" si="2"/>
+        <f>E31/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F75" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>F31/d4_tot</f>
+        <v>0.25</v>
       </c>
       <c r="G75" s="5">
-        <f t="shared" si="4"/>
-        <v>0.14285714285714285</v>
+        <f>G31/d5_tot</f>
+        <v>0</v>
       </c>
       <c r="H75" s="5">
-        <f t="shared" si="5"/>
+        <f>H31/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I75" s="5">
-        <f t="shared" si="6"/>
+        <f>I31/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J75" s="5">
-        <f t="shared" si="7"/>
+        <f>J31/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K75" s="5">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="L75" s="5">
-        <f>C75*K75</f>
-        <v>0.2857142857142857</v>
-      </c>
+        <f>LN(8/K31)</f>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L75" s="5"/>
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C76" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>C32/d1_tot</f>
+        <v>0.2</v>
       </c>
       <c r="D76" s="5">
-        <f t="shared" si="9"/>
+        <f>D32/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E76" s="5">
-        <f t="shared" si="2"/>
+        <f>E32/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F76" s="5">
-        <f t="shared" si="3"/>
+        <f>F32/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G76" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>G32/d5_tot</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H76" s="5">
-        <f t="shared" si="5"/>
+        <f>H32/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I76" s="5">
-        <f t="shared" si="6"/>
+        <f>I32/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J76" s="5">
-        <f t="shared" si="7"/>
-        <v>0.2</v>
+        <f>J32/d8_tot</f>
+        <v>0</v>
       </c>
       <c r="K76" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="L76" s="5"/>
+        <f>LN(8/K32)</f>
+        <v>1.3862943611198906</v>
+      </c>
+      <c r="L76" s="5">
+        <f>C76*K76</f>
+        <v>0.2772588722239781</v>
+      </c>
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="5"/>
       <c r="B77" s="5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C77" s="5">
-        <f t="shared" si="8"/>
+        <f>C33/d1_tot</f>
         <v>0</v>
       </c>
       <c r="D77" s="5">
-        <f t="shared" si="9"/>
-        <v>0.16666666666666666</v>
+        <f>D33/d2_tot</f>
+        <v>0</v>
       </c>
       <c r="E77" s="5">
-        <f t="shared" si="2"/>
+        <f>E33/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F77" s="5">
-        <f t="shared" si="3"/>
+        <f>F33/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G77" s="5">
-        <f t="shared" si="4"/>
+        <f>G33/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H77" s="5">
-        <f t="shared" si="5"/>
+        <f>H33/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I77" s="5">
-        <f t="shared" si="6"/>
+        <f>I33/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J77" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>J33/d8_tot</f>
+        <v>0.25</v>
       </c>
       <c r="K77" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>LN(8/K33)</f>
+        <v>2.0794415416798357</v>
       </c>
       <c r="L77" s="5"/>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C78" s="5">
-        <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
+        <f>C34/d1_tot</f>
+        <v>0</v>
       </c>
       <c r="D78" s="5">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>D34/d2_tot</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E78" s="5">
-        <f t="shared" si="2"/>
+        <f>E34/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F78" s="5">
-        <f t="shared" si="3"/>
+        <f>F34/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G78" s="5">
-        <f t="shared" si="4"/>
+        <f>G34/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H78" s="5">
-        <f t="shared" si="5"/>
+        <f>H34/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I78" s="5">
-        <f t="shared" si="6"/>
+        <f>I34/d7_tot</f>
         <v>0</v>
       </c>
       <c r="J78" s="5">
-        <f t="shared" si="7"/>
+        <f>J34/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K78" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="L78" s="5">
-        <f>C78*K78</f>
-        <v>0.42857142857142855</v>
-      </c>
+        <f>LN(8/K34)</f>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L78" s="5"/>
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C79" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>C35/d1_tot</f>
+        <v>0.2</v>
       </c>
       <c r="D79" s="5">
-        <f t="shared" si="9"/>
+        <f>D35/d2_tot</f>
         <v>0</v>
       </c>
       <c r="E79" s="5">
-        <f t="shared" si="2"/>
+        <f>E35/d3_tot</f>
         <v>0</v>
       </c>
       <c r="F79" s="5">
-        <f t="shared" si="3"/>
+        <f>F35/d4_tot</f>
         <v>0</v>
       </c>
       <c r="G79" s="5">
-        <f t="shared" si="4"/>
+        <f>G35/d5_tot</f>
         <v>0</v>
       </c>
       <c r="H79" s="5">
-        <f t="shared" si="5"/>
+        <f>H35/d6_tot</f>
         <v>0</v>
       </c>
       <c r="I79" s="5">
-        <f t="shared" si="6"/>
-        <v>0.125</v>
+        <f>I35/d7_tot</f>
+        <v>0</v>
       </c>
       <c r="J79" s="5">
-        <f t="shared" si="7"/>
+        <f>J35/d8_tot</f>
         <v>0</v>
       </c>
       <c r="K79" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="L79" s="5"/>
+        <f>LN(8/K35)</f>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L79" s="5">
+        <f>C79*K79</f>
+        <v>0.41588830833596718</v>
+      </c>
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="5"/>
       <c r="B80" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C80" s="5">
+        <f>C36/d1_tot</f>
+        <v>0</v>
+      </c>
+      <c r="D80" s="5">
+        <f>D36/d2_tot</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="5">
+        <f>E36/d3_tot</f>
+        <v>0</v>
+      </c>
+      <c r="F80" s="5">
+        <f>F36/d4_tot</f>
+        <v>0</v>
+      </c>
+      <c r="G80" s="5">
+        <f>G36/d5_tot</f>
+        <v>0</v>
+      </c>
+      <c r="H80" s="5">
+        <f>H36/d6_tot</f>
+        <v>0</v>
+      </c>
+      <c r="I80" s="5">
+        <f>I36/d7_tot</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J80" s="5">
+        <f>J36/d8_tot</f>
+        <v>0</v>
+      </c>
+      <c r="K80" s="5">
+        <f>LN(8/K36)</f>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L80" s="5"/>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C80" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D80" s="5">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E80" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F80" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G80" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H80" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I80" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J80" s="5">
-        <f t="shared" si="7"/>
-        <v>0.2</v>
-      </c>
-      <c r="K80" s="5">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="L80" s="5"/>
-    </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="1" t="s">
+      <c r="C81" s="5">
+        <f>C37/d1_tot</f>
+        <v>0</v>
+      </c>
+      <c r="D81" s="5">
+        <f>D37/d2_tot</f>
+        <v>0</v>
+      </c>
+      <c r="E81" s="5">
+        <f>E37/d3_tot</f>
+        <v>0</v>
+      </c>
+      <c r="F81" s="5">
+        <f>F37/d4_tot</f>
+        <v>0</v>
+      </c>
+      <c r="G81" s="5">
+        <f>G37/d5_tot</f>
+        <v>0</v>
+      </c>
+      <c r="H81" s="5">
+        <f>H37/d6_tot</f>
+        <v>0</v>
+      </c>
+      <c r="I81" s="5">
+        <f>I37/d7_tot</f>
+        <v>0</v>
+      </c>
+      <c r="J81" s="5">
+        <f>J37/d8_tot</f>
+        <v>0.25</v>
+      </c>
+      <c r="K81" s="5">
+        <f>LN(8/K37)</f>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="L81" s="5"/>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B81" s="1">
-        <f>COUNTA(B46:B80)</f>
+      <c r="B82" s="6">
+        <f>COUNTA(B47:B81)</f>
         <v>35</v>
       </c>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
     </row>
   </sheetData>
   <sortState ref="B3:J37">
@@ -3255,10 +3256,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24037F83-76E3-AE4B-B56D-9DECCA96923C}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A15" sqref="A15:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3304,6 +3305,16 @@
         <v>91</v>
       </c>
     </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>